<commit_message>
User Navigation, Report currency BYN
</commit_message>
<xml_diff>
--- a/Thesis/Bill.xlsx
+++ b/Thesis/Bill.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mi\source\repos\Thesis\Thesis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59949275-D55B-440C-8D0C-F89633F4DEFA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33DD2A68-3392-45E2-B0CD-6F1AAF10BE15}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2730" yWindow="450" windowWidth="23265" windowHeight="15300" tabRatio="187" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1170" yWindow="450" windowWidth="23265" windowHeight="15300" tabRatio="187" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Накладная" sheetId="1" r:id="rId1"/>
@@ -55,10 +55,10 @@
     <t>Чек № 0000000</t>
   </si>
   <si>
-    <t>Цена</t>
+    <t>Цена, BYN</t>
   </si>
   <si>
-    <t>Сумма</t>
+    <t>Сумма, BYN</t>
   </si>
 </sst>
 </file>
@@ -283,7 +283,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -295,23 +295,14 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="2" fontId="5" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -331,21 +322,6 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -355,8 +331,29 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -712,37 +709,37 @@
   <sheetData>
     <row r="1" spans="1:36" s="1" customFormat="1" ht="11.25" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="2" spans="1:36" s="1" customFormat="1" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="23" t="s">
+      <c r="A2" s="15" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="23"/>
-      <c r="C2" s="23"/>
-      <c r="D2" s="23"/>
-      <c r="E2" s="23"/>
-      <c r="F2" s="23"/>
-      <c r="G2" s="23"/>
-      <c r="H2" s="23"/>
-      <c r="I2" s="23"/>
-      <c r="J2" s="23"/>
-      <c r="K2" s="23"/>
-      <c r="L2" s="23"/>
-      <c r="M2" s="23"/>
-      <c r="N2" s="23"/>
-      <c r="O2" s="23"/>
-      <c r="P2" s="23"/>
-      <c r="Q2" s="23"/>
-      <c r="R2" s="23"/>
-      <c r="S2" s="23"/>
-      <c r="T2" s="23"/>
-      <c r="U2" s="23"/>
-      <c r="V2" s="23"/>
-      <c r="W2" s="23"/>
-      <c r="X2" s="23"/>
-      <c r="Y2" s="23"/>
-      <c r="Z2" s="23"/>
-      <c r="AA2" s="23"/>
-      <c r="AB2" s="23"/>
-      <c r="AC2" s="7"/>
+      <c r="B2" s="15"/>
+      <c r="C2" s="15"/>
+      <c r="D2" s="15"/>
+      <c r="E2" s="15"/>
+      <c r="F2" s="15"/>
+      <c r="G2" s="15"/>
+      <c r="H2" s="15"/>
+      <c r="I2" s="15"/>
+      <c r="J2" s="15"/>
+      <c r="K2" s="15"/>
+      <c r="L2" s="15"/>
+      <c r="M2" s="15"/>
+      <c r="N2" s="15"/>
+      <c r="O2" s="15"/>
+      <c r="P2" s="15"/>
+      <c r="Q2" s="15"/>
+      <c r="R2" s="15"/>
+      <c r="S2" s="15"/>
+      <c r="T2" s="15"/>
+      <c r="U2" s="15"/>
+      <c r="V2" s="15"/>
+      <c r="W2" s="15"/>
+      <c r="X2" s="15"/>
+      <c r="Y2" s="15"/>
+      <c r="Z2" s="15"/>
+      <c r="AA2" s="15"/>
+      <c r="AB2" s="15"/>
+      <c r="AC2" s="6"/>
     </row>
     <row r="3" spans="1:36" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="AC3" s="2"/>
@@ -755,37 +752,37 @@
       <c r="AJ3"/>
     </row>
     <row r="4" spans="1:36" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="22" t="s">
+      <c r="A4" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="B4" s="22"/>
-      <c r="C4" s="22"/>
-      <c r="D4" s="22"/>
-      <c r="E4" s="22"/>
-      <c r="F4" s="24"/>
-      <c r="G4" s="24"/>
-      <c r="H4" s="24"/>
-      <c r="I4" s="24"/>
-      <c r="J4" s="24"/>
-      <c r="K4" s="24"/>
-      <c r="L4" s="24"/>
-      <c r="M4" s="24"/>
-      <c r="N4" s="24"/>
-      <c r="O4" s="24"/>
-      <c r="P4" s="24"/>
-      <c r="Q4" s="24"/>
-      <c r="R4" s="24"/>
-      <c r="S4" s="24"/>
-      <c r="T4" s="24"/>
-      <c r="U4" s="24"/>
-      <c r="V4" s="24"/>
-      <c r="W4" s="24"/>
-      <c r="X4" s="24"/>
-      <c r="Y4" s="24"/>
-      <c r="Z4" s="24"/>
-      <c r="AA4" s="24"/>
-      <c r="AB4" s="24"/>
-      <c r="AC4" s="6"/>
+      <c r="B4" s="14"/>
+      <c r="C4" s="14"/>
+      <c r="D4" s="14"/>
+      <c r="E4" s="14"/>
+      <c r="F4" s="16"/>
+      <c r="G4" s="16"/>
+      <c r="H4" s="16"/>
+      <c r="I4" s="16"/>
+      <c r="J4" s="16"/>
+      <c r="K4" s="16"/>
+      <c r="L4" s="16"/>
+      <c r="M4" s="16"/>
+      <c r="N4" s="16"/>
+      <c r="O4" s="16"/>
+      <c r="P4" s="16"/>
+      <c r="Q4" s="16"/>
+      <c r="R4" s="16"/>
+      <c r="S4" s="16"/>
+      <c r="T4" s="16"/>
+      <c r="U4" s="16"/>
+      <c r="V4" s="16"/>
+      <c r="W4" s="16"/>
+      <c r="X4" s="16"/>
+      <c r="Y4" s="16"/>
+      <c r="Z4" s="16"/>
+      <c r="AA4" s="16"/>
+      <c r="AB4" s="16"/>
+      <c r="AC4" s="5"/>
       <c r="AD4"/>
       <c r="AE4"/>
       <c r="AF4"/>
@@ -796,37 +793,37 @@
     </row>
     <row r="5" spans="1:36" s="1" customFormat="1" ht="7.15" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="6" spans="1:36" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="22" t="s">
+      <c r="A6" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="B6" s="22"/>
-      <c r="C6" s="22"/>
-      <c r="D6" s="22"/>
-      <c r="E6" s="22"/>
-      <c r="F6" s="24"/>
-      <c r="G6" s="24"/>
-      <c r="H6" s="24"/>
-      <c r="I6" s="24"/>
-      <c r="J6" s="24"/>
-      <c r="K6" s="24"/>
-      <c r="L6" s="24"/>
-      <c r="M6" s="24"/>
-      <c r="N6" s="24"/>
-      <c r="O6" s="24"/>
-      <c r="P6" s="24"/>
-      <c r="Q6" s="24"/>
-      <c r="R6" s="24"/>
-      <c r="S6" s="24"/>
-      <c r="T6" s="24"/>
-      <c r="U6" s="24"/>
-      <c r="V6" s="24"/>
-      <c r="W6" s="24"/>
-      <c r="X6" s="24"/>
-      <c r="Y6" s="24"/>
-      <c r="Z6" s="24"/>
-      <c r="AA6" s="24"/>
-      <c r="AB6" s="24"/>
-      <c r="AC6" s="6"/>
+      <c r="B6" s="14"/>
+      <c r="C6" s="14"/>
+      <c r="D6" s="14"/>
+      <c r="E6" s="14"/>
+      <c r="F6" s="16"/>
+      <c r="G6" s="16"/>
+      <c r="H6" s="16"/>
+      <c r="I6" s="16"/>
+      <c r="J6" s="16"/>
+      <c r="K6" s="16"/>
+      <c r="L6" s="16"/>
+      <c r="M6" s="16"/>
+      <c r="N6" s="16"/>
+      <c r="O6" s="16"/>
+      <c r="P6" s="16"/>
+      <c r="Q6" s="16"/>
+      <c r="R6" s="16"/>
+      <c r="S6" s="16"/>
+      <c r="T6" s="16"/>
+      <c r="U6" s="16"/>
+      <c r="V6" s="16"/>
+      <c r="W6" s="16"/>
+      <c r="X6" s="16"/>
+      <c r="Y6" s="16"/>
+      <c r="Z6" s="16"/>
+      <c r="AA6" s="16"/>
+      <c r="AB6" s="16"/>
+      <c r="AC6" s="5"/>
       <c r="AG6"/>
       <c r="AH6"/>
       <c r="AI6"/>
@@ -834,34 +831,34 @@
     </row>
     <row r="7" spans="1:36" s="1" customFormat="1" ht="7.15" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="8" spans="1:36" ht="7.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="11"/>
-      <c r="B8" s="11"/>
-      <c r="C8" s="11"/>
-      <c r="D8" s="11"/>
-      <c r="E8" s="11"/>
-      <c r="F8" s="6"/>
-      <c r="G8" s="6"/>
-      <c r="H8" s="6"/>
-      <c r="I8" s="6"/>
-      <c r="J8" s="6"/>
-      <c r="K8" s="6"/>
-      <c r="L8" s="6"/>
-      <c r="M8" s="6"/>
-      <c r="N8" s="6"/>
-      <c r="O8" s="6"/>
-      <c r="P8" s="6"/>
-      <c r="Q8" s="6"/>
-      <c r="R8" s="6"/>
-      <c r="S8" s="6"/>
-      <c r="T8" s="6"/>
-      <c r="U8" s="6"/>
-      <c r="V8" s="6"/>
-      <c r="W8" s="6"/>
-      <c r="X8" s="6"/>
-      <c r="Y8" s="6"/>
-      <c r="Z8" s="6"/>
-      <c r="AA8" s="6"/>
-      <c r="AB8" s="6"/>
+      <c r="A8" s="8"/>
+      <c r="B8" s="8"/>
+      <c r="C8" s="8"/>
+      <c r="D8" s="8"/>
+      <c r="E8" s="8"/>
+      <c r="F8" s="5"/>
+      <c r="G8" s="5"/>
+      <c r="H8" s="5"/>
+      <c r="I8" s="5"/>
+      <c r="J8" s="5"/>
+      <c r="K8" s="5"/>
+      <c r="L8" s="5"/>
+      <c r="M8" s="5"/>
+      <c r="N8" s="5"/>
+      <c r="O8" s="5"/>
+      <c r="P8" s="5"/>
+      <c r="Q8" s="5"/>
+      <c r="R8" s="5"/>
+      <c r="S8" s="5"/>
+      <c r="T8" s="5"/>
+      <c r="U8" s="5"/>
+      <c r="V8" s="5"/>
+      <c r="W8" s="5"/>
+      <c r="X8" s="5"/>
+      <c r="Y8" s="5"/>
+      <c r="Z8" s="5"/>
+      <c r="AA8" s="5"/>
+      <c r="AB8" s="5"/>
       <c r="AC8"/>
       <c r="AD8"/>
       <c r="AE8"/>
@@ -873,43 +870,43 @@
     </row>
     <row r="9" spans="1:36" s="1" customFormat="1" ht="8.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="10" spans="1:36" ht="24.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="15" t="s">
+      <c r="A10" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="B10" s="15"/>
-      <c r="C10" s="16" t="s">
+      <c r="B10" s="12"/>
+      <c r="C10" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="D10" s="16"/>
-      <c r="E10" s="16"/>
-      <c r="F10" s="16"/>
-      <c r="G10" s="12" t="s">
+      <c r="D10" s="13"/>
+      <c r="E10" s="13"/>
+      <c r="F10" s="13"/>
+      <c r="G10" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="H10" s="13"/>
-      <c r="I10" s="13"/>
-      <c r="J10" s="13"/>
-      <c r="K10" s="13"/>
-      <c r="L10" s="13"/>
-      <c r="M10" s="13"/>
-      <c r="N10" s="14"/>
-      <c r="O10" s="12" t="s">
+      <c r="H10" s="10"/>
+      <c r="I10" s="10"/>
+      <c r="J10" s="10"/>
+      <c r="K10" s="10"/>
+      <c r="L10" s="10"/>
+      <c r="M10" s="10"/>
+      <c r="N10" s="11"/>
+      <c r="O10" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="P10" s="13"/>
-      <c r="Q10" s="13"/>
-      <c r="R10" s="13"/>
-      <c r="S10" s="13"/>
-      <c r="T10" s="13"/>
-      <c r="U10" s="14"/>
-      <c r="V10" s="12" t="s">
+      <c r="P10" s="10"/>
+      <c r="Q10" s="10"/>
+      <c r="R10" s="10"/>
+      <c r="S10" s="10"/>
+      <c r="T10" s="10"/>
+      <c r="U10" s="11"/>
+      <c r="V10" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="W10" s="13"/>
-      <c r="X10" s="13"/>
-      <c r="Y10" s="13"/>
-      <c r="Z10" s="13"/>
-      <c r="AA10" s="14"/>
+      <c r="W10" s="10"/>
+      <c r="X10" s="10"/>
+      <c r="Y10" s="10"/>
+      <c r="Z10" s="10"/>
+      <c r="AA10" s="11"/>
       <c r="AB10" s="3" t="s">
         <v>8</v>
       </c>
@@ -946,14 +943,14 @@
       <c r="S11" s="20"/>
       <c r="T11" s="20"/>
       <c r="U11" s="21"/>
-      <c r="V11" s="8"/>
-      <c r="W11" s="9"/>
-      <c r="X11" s="9"/>
-      <c r="Y11" s="9"/>
-      <c r="Z11" s="9"/>
-      <c r="AA11" s="10"/>
-      <c r="AB11" s="5"/>
-      <c r="AC11" s="25"/>
+      <c r="V11" s="22"/>
+      <c r="W11" s="23"/>
+      <c r="X11" s="23"/>
+      <c r="Y11" s="23"/>
+      <c r="Z11" s="23"/>
+      <c r="AA11" s="24"/>
+      <c r="AB11" s="7"/>
+      <c r="AC11" s="7"/>
       <c r="AD11"/>
       <c r="AE11"/>
       <c r="AF11"/>

</xml_diff>